<commit_message>
Modified external_query, medical_query, excel and internal_query
</commit_message>
<xml_diff>
--- a/lifeEase - Personal Input Sheet.xlsx
+++ b/lifeEase - Personal Input Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Purvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purvi/Desktop/boaient/OpenAI model - lifeCare Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B3CF68-5F1D-499B-947B-BBBDF1E7F86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7141AC23-667D-5048-9473-58253F54C7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62917026-952F-4E83-BA4F-B38EECD54274}"/>
+    <workbookView xWindow="2000" yWindow="1540" windowWidth="30240" windowHeight="17720" xr2:uid="{62917026-952F-4E83-BA4F-B38EECD54274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
   <si>
     <t>Category</t>
   </si>
@@ -53,36 +53,21 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Maya</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Vyas</t>
-  </si>
-  <si>
     <t>Childhood Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Sandhya </t>
-  </si>
-  <si>
     <t>Known by other Names</t>
   </si>
   <si>
-    <t>Shakuntala</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t>Privacy Preferences</t>
   </si>
   <si>
-    <t>Husband and Daughter death</t>
-  </si>
-  <si>
     <t>Favorite Foods</t>
   </si>
   <si>
@@ -552,6 +534,21 @@
   </si>
   <si>
     <t>Any Other Relevant Personal Information</t>
+  </si>
+  <si>
+    <t>Vishnu</t>
+  </si>
+  <si>
+    <t>Prasad</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>23.08.1970</t>
+  </si>
+  <si>
+    <t>Father death</t>
   </si>
 </sst>
 </file>
@@ -958,18 +955,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924498B4-15F6-4D2C-B171-A7E794AD6524}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="46.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -988,796 +985,793 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>17898</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C30" s="6">
         <v>7.15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C31" s="6">
         <v>10.15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1786,6 +1780,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D4E9A7986190449970A1787155DD3C1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="04f971603dee42d7177a8f4d04d6cdac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00e1dc6d-086e-49e7-bf0a-251e212c2c32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="804fe28716a63320b9b690431aeb42eb" ns2:_="">
     <xsd:import namespace="00e1dc6d-086e-49e7-bf0a-251e212c2c32"/>
@@ -1929,22 +1938,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2B604D3-D29F-4F0E-A337-95A02F8255CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92053FB6-7139-4D87-B63E-1222BB1282B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80035DA4-93F7-4BFC-B9CE-A7DC8740EFF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1960,21 +1971,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2B604D3-D29F-4F0E-A337-95A02F8255CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92053FB6-7139-4D87-B63E-1222BB1282B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>